<commit_message>
update 18 files, create 1 file and delete 8 files
</commit_message>
<xml_diff>
--- a/rivtManual/solar-canopy-2023/rivt-solar-canopy/rv0101-project-overview/data/cbc2019_stds.xlsx
+++ b/rivtManual/solar-canopy-2023/rivt-solar-canopy/rv0101-project-overview/data/cbc2019_stds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\projects\residence_remodel\rivtcalcs\calcs\c0101\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\solar_canopy\rivtManual\solar-canopy-2023\rivt-solar-canopy\rv0101-project-overview\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EB21B3-6D93-4F0A-BDB7-0AB8BE6C36E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62BD716-0E58-4009-9692-A26B40D17180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Loading</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Year</t>
-  </si>
-  <si>
-    <t>CBC 2019 - Structural Reference Standards</t>
   </si>
   <si>
     <t>AWC-SDPWS</t>
@@ -105,14 +102,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,87 +446,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="50.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="50.15625" customWidth="1"/>
+    <col min="2" max="2" width="21.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C5">
+        <v>2015</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="C6">
         <v>2018</v>
       </c>
     </row>
@@ -547,7 +536,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -559,7 +548,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>